<commit_message>
Completed Executive Summary, Gap Analysis, and POA&M.
</commit_message>
<xml_diff>
--- a/CMMC-Demo-Aegis-Avionics/Gap-Assessment.xlsx
+++ b/CMMC-Demo-Aegis-Avionics/Gap-Assessment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikael\Biz\NIST-800-171-Readiness-Assessment\CMMC-Demo-Aegis-Avionics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E05584F-6FFD-417B-BD49-4B11C86F36CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8B459C-E590-460C-97E4-6E238CA7C1F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{0AC88B97-F9F5-4B13-A825-936F26B68506}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="106">
   <si>
     <t>Control ID</t>
   </si>
@@ -156,6 +156,204 @@
   </si>
   <si>
     <t>Increases risk of privilege misuse or compromise.</t>
+  </si>
+  <si>
+    <t>AC 3.1.7</t>
+  </si>
+  <si>
+    <t>Prevent non-privileged users from executing privileged functions</t>
+  </si>
+  <si>
+    <t>Endpoint configuration samples, Intune policy overview</t>
+  </si>
+  <si>
+    <t>Standard users are restricted from executing most priviliged functions; however, inconsistent local admin rights weaken enforcement of this control</t>
+  </si>
+  <si>
+    <t>Unauthorized system changes may occur on endpoints with elevated user privileges</t>
+  </si>
+  <si>
+    <t>AC 3.1.8</t>
+  </si>
+  <si>
+    <t>Limit unsuccessful logon attempts</t>
+  </si>
+  <si>
+    <t>Implemented</t>
+  </si>
+  <si>
+    <t>Entra ID security defaults, MFA enforcement</t>
+  </si>
+  <si>
+    <t>Account lockout and authentication protections are enforced through Entra ID security defaults and MFA configurations.</t>
+  </si>
+  <si>
+    <t>Low residual risk related to brute-force authentication attempts</t>
+  </si>
+  <si>
+    <t>AC 3.1.9</t>
+  </si>
+  <si>
+    <t>Provide privacy and security notices upon access</t>
+  </si>
+  <si>
+    <t>Endpoint login screen review, policy documentation</t>
+  </si>
+  <si>
+    <t>No system use or security warning banners are displayed during user login to endpoints or cloud services</t>
+  </si>
+  <si>
+    <t>Lack of user notification weakens legan and policy enforcemen</t>
+  </si>
+  <si>
+    <t>AC 3.1.10</t>
+  </si>
+  <si>
+    <t>Use session lock after inactivity</t>
+  </si>
+  <si>
+    <t>Intune device compliance policy samples</t>
+  </si>
+  <si>
+    <t>Session lock settings are configured on some managed endpoints;however policies are not consistently enforced across all devices.</t>
+  </si>
+  <si>
+    <t>Unlock systems may be accessed by unauthorized individuals</t>
+  </si>
+  <si>
+    <t>AC 3.1.11</t>
+  </si>
+  <si>
+    <t>Terminate sessions after defined conditions</t>
+  </si>
+  <si>
+    <t>Conditional Access Policy overview</t>
+  </si>
+  <si>
+    <t>Session  termination is enforced through cloud session controls; however, timeout values are not formally documented or reviewed</t>
+  </si>
+  <si>
+    <t>Extended sessions increase exposure window if accounts are compromised</t>
+  </si>
+  <si>
+    <t>AC 3.1.12</t>
+  </si>
+  <si>
+    <t>Monitor and control remote access sessions</t>
+  </si>
+  <si>
+    <t>VPN configuration review, Conditional Access Policies</t>
+  </si>
+  <si>
+    <t>Remote access is controlled via VPN and conditional access; however, monitoring and logging of remote sessions are limited and not routinely reviewed</t>
+  </si>
+  <si>
+    <t>Unauthorized or anomalous remote access activity may go undetected</t>
+  </si>
+  <si>
+    <t>AC 3.1.13</t>
+  </si>
+  <si>
+    <t>Employ cryptographic mechanisms to protect remote access sessions</t>
+  </si>
+  <si>
+    <t>VPN encryption msettings, HTTPS/TLS configuration</t>
+  </si>
+  <si>
+    <t>Remote access sessions are protected using encrypted VPN tunnels and TLS-protected cloud services</t>
+  </si>
+  <si>
+    <t>Low residual risk related to interception of remote access traffic</t>
+  </si>
+  <si>
+    <t>AC 3.1.14</t>
+  </si>
+  <si>
+    <t>Route remote access via managed access control points</t>
+  </si>
+  <si>
+    <t>Network firewall configuration, VPN architecture overview</t>
+  </si>
+  <si>
+    <t>Remote access to the CUI environment is routed through managed VPN and firewall infrastructure</t>
+  </si>
+  <si>
+    <t>Low risk provided configrations reamin maintained</t>
+  </si>
+  <si>
+    <t>AC 3.1.15</t>
+  </si>
+  <si>
+    <t>Authorize remote execution of privileged commands</t>
+  </si>
+  <si>
+    <t>Interview notes, administrative access review</t>
+  </si>
+  <si>
+    <t>No formal authorization or documentation exists governing remote execution of privileged commands</t>
+  </si>
+  <si>
+    <t>Elevated risk of unauthorized or undocumented administrative actions</t>
+  </si>
+  <si>
+    <t>AC 3.1.16</t>
+  </si>
+  <si>
+    <t>Authorize wireless access prior to connection</t>
+  </si>
+  <si>
+    <t>Wi-Fi configuration review, network interview</t>
+  </si>
+  <si>
+    <t>Corporate wireless access requires authentication; however, device authorization and network segmentation controls are not fully documented</t>
+  </si>
+  <si>
+    <t>Unauthorized devices may gain access to internal networks</t>
+  </si>
+  <si>
+    <t>AC 3.1.17</t>
+  </si>
+  <si>
+    <t>Protect wireless access using authentication and encryption</t>
+  </si>
+  <si>
+    <t>Wireless security configuration</t>
+  </si>
+  <si>
+    <t>Wireless networks employ encrypted protocols and authentication mechanisms</t>
+  </si>
+  <si>
+    <t>Low residual risk if configurations remain enforced</t>
+  </si>
+  <si>
+    <t>AC 3.1.18</t>
+  </si>
+  <si>
+    <t>Control connection of mobile devices</t>
+  </si>
+  <si>
+    <t>Mobile device access review, policy documentation</t>
+  </si>
+  <si>
+    <t>Mobile access to M365 is permitted; however, mobile device management and enforcement of security controls are limited.</t>
+  </si>
+  <si>
+    <t>CUI may be accessed on devices lacking sufficient security controls</t>
+  </si>
+  <si>
+    <t>AC 3.1.19</t>
+  </si>
+  <si>
+    <t>Encrypt CUI on mobile devices and mobile computing platforms</t>
+  </si>
+  <si>
+    <t>Device encryption samples, policy review</t>
+  </si>
+  <si>
+    <t>Device encryption is enabled on most company-managed laptops; however, enforcement and verification are inconsistent, particularly for mobile devices.</t>
+  </si>
+  <si>
+    <t>Risk of CUI exposure if devices are lost or stolen</t>
   </si>
 </sst>
 </file>
@@ -543,10 +741,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BF6A127-B510-4145-88BF-55E8C342B462}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B6" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -721,6 +920,305 @@
         <v>39</v>
       </c>
     </row>
+    <row r="8" spans="1:7" ht="142.5">
+      <c r="A8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="99.75">
+      <c r="A9" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="99.75">
+      <c r="A10" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="128.25">
+      <c r="A11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C11" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="128.25">
+      <c r="A12" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="128.25">
+      <c r="A13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="99.75">
+      <c r="A14" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" t="s">
+        <v>47</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="99.75">
+      <c r="A15" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="G15" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="99.75">
+      <c r="A16" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" t="s">
+        <v>26</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="128.25">
+      <c r="A17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="71.25">
+      <c r="A18" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="114">
+      <c r="A19" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19" t="s">
+        <v>9</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="128.25">
+      <c r="A20" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C20" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>9</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>